<commit_message>
fix: upload 211a baru dengan formulae
</commit_message>
<xml_diff>
--- a/public/exports/PG211A.xlsx
+++ b/public/exports/PG211A.xlsx
@@ -1459,7 +1459,10 @@
       <c r="B13" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="33"/>
+      <c r="C13" s="33">
+        <f t="shared" ref="C13:C48" si="1">SUM(D13:E13)</f>
+        <v>0</v>
+      </c>
       <c r="D13" s="34"/>
       <c r="E13" s="34"/>
       <c r="F13" s="35"/>
@@ -1497,7 +1500,10 @@
       <c r="B14" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="39"/>
+      <c r="C14" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D14" s="40"/>
       <c r="E14" s="40"/>
       <c r="F14" s="41"/>
@@ -1537,7 +1543,10 @@
       <c r="B15" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="33"/>
+      <c r="C15" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D15" s="34"/>
       <c r="E15" s="38"/>
       <c r="F15" s="47"/>
@@ -1575,7 +1584,10 @@
       <c r="B16" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="39"/>
+      <c r="C16" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D16" s="40"/>
       <c r="E16" s="44"/>
       <c r="F16" s="41"/>
@@ -1615,7 +1627,10 @@
       <c r="B17" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="33"/>
+      <c r="C17" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D17" s="34"/>
       <c r="E17" s="38"/>
       <c r="F17" s="47"/>
@@ -1653,7 +1668,10 @@
       <c r="B18" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="39"/>
+      <c r="C18" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D18" s="40"/>
       <c r="E18" s="44"/>
       <c r="F18" s="41"/>
@@ -1693,7 +1711,10 @@
       <c r="B19" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="33"/>
+      <c r="C19" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D19" s="34"/>
       <c r="E19" s="38"/>
       <c r="F19" s="47"/>
@@ -1731,7 +1752,10 @@
       <c r="B20" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="39"/>
+      <c r="C20" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D20" s="44"/>
       <c r="E20" s="44"/>
       <c r="F20" s="41"/>
@@ -1771,7 +1795,10 @@
       <c r="B21" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="33"/>
+      <c r="C21" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D21" s="38"/>
       <c r="E21" s="38"/>
       <c r="F21" s="47"/>
@@ -1809,7 +1836,10 @@
       <c r="B22" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="39"/>
+      <c r="C22" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D22" s="44"/>
       <c r="E22" s="44"/>
       <c r="F22" s="41"/>
@@ -1849,7 +1879,10 @@
       <c r="B23" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="33"/>
+      <c r="C23" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D23" s="38"/>
       <c r="E23" s="38"/>
       <c r="F23" s="47"/>
@@ -1887,7 +1920,10 @@
       <c r="B24" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="39"/>
+      <c r="C24" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D24" s="44"/>
       <c r="E24" s="44"/>
       <c r="F24" s="41"/>
@@ -1927,7 +1963,10 @@
       <c r="B25" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="33"/>
+      <c r="C25" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D25" s="38"/>
       <c r="E25" s="38"/>
       <c r="F25" s="35"/>
@@ -1965,7 +2004,10 @@
       <c r="B26" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="39"/>
+      <c r="C26" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D26" s="44"/>
       <c r="E26" s="44"/>
       <c r="F26" s="41"/>
@@ -2005,7 +2047,10 @@
       <c r="B27" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="33"/>
+      <c r="C27" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D27" s="38"/>
       <c r="E27" s="38"/>
       <c r="F27" s="35"/>
@@ -2043,7 +2088,10 @@
       <c r="B28" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="39"/>
+      <c r="C28" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D28" s="44"/>
       <c r="E28" s="44"/>
       <c r="F28" s="41"/>
@@ -2083,7 +2131,10 @@
       <c r="B29" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="33"/>
+      <c r="C29" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D29" s="38"/>
       <c r="E29" s="38"/>
       <c r="F29" s="35"/>
@@ -2121,7 +2172,10 @@
       <c r="B30" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="39"/>
+      <c r="C30" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D30" s="44"/>
       <c r="E30" s="44"/>
       <c r="F30" s="41"/>
@@ -2161,7 +2215,10 @@
       <c r="B31" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="33"/>
+      <c r="C31" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D31" s="38"/>
       <c r="E31" s="38"/>
       <c r="F31" s="35"/>
@@ -2199,7 +2256,10 @@
       <c r="B32" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="39"/>
+      <c r="C32" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D32" s="44"/>
       <c r="E32" s="44"/>
       <c r="F32" s="41"/>
@@ -2239,7 +2299,10 @@
       <c r="B33" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="33"/>
+      <c r="C33" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D33" s="38"/>
       <c r="E33" s="38"/>
       <c r="F33" s="35"/>
@@ -2277,7 +2340,10 @@
       <c r="B34" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="39"/>
+      <c r="C34" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D34" s="44"/>
       <c r="E34" s="44"/>
       <c r="F34" s="41"/>
@@ -2317,7 +2383,10 @@
       <c r="B35" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="33"/>
+      <c r="C35" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D35" s="38"/>
       <c r="E35" s="38"/>
       <c r="F35" s="35"/>
@@ -2355,7 +2424,10 @@
       <c r="B36" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="39"/>
+      <c r="C36" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D36" s="44"/>
       <c r="E36" s="44"/>
       <c r="F36" s="41"/>
@@ -2395,7 +2467,10 @@
       <c r="B37" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="33"/>
+      <c r="C37" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D37" s="38"/>
       <c r="E37" s="38"/>
       <c r="F37" s="35"/>
@@ -2433,7 +2508,10 @@
       <c r="B38" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="39"/>
+      <c r="C38" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D38" s="44"/>
       <c r="E38" s="44"/>
       <c r="F38" s="41"/>
@@ -2473,7 +2551,10 @@
       <c r="B39" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="33"/>
+      <c r="C39" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D39" s="38"/>
       <c r="E39" s="38"/>
       <c r="F39" s="34"/>
@@ -2511,7 +2592,10 @@
       <c r="B40" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C40" s="39"/>
+      <c r="C40" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D40" s="44"/>
       <c r="E40" s="44"/>
       <c r="F40" s="41"/>
@@ -2551,7 +2635,10 @@
       <c r="B41" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C41" s="33"/>
+      <c r="C41" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D41" s="38"/>
       <c r="E41" s="38"/>
       <c r="F41" s="34"/>
@@ -2589,7 +2676,10 @@
       <c r="B42" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C42" s="39"/>
+      <c r="C42" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D42" s="44"/>
       <c r="E42" s="44"/>
       <c r="F42" s="41"/>
@@ -2629,7 +2719,10 @@
       <c r="B43" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C43" s="33"/>
+      <c r="C43" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D43" s="38"/>
       <c r="E43" s="38"/>
       <c r="F43" s="34"/>
@@ -2667,7 +2760,10 @@
       <c r="B44" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C44" s="39"/>
+      <c r="C44" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D44" s="44"/>
       <c r="E44" s="44"/>
       <c r="F44" s="41"/>
@@ -2707,7 +2803,10 @@
       <c r="B45" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C45" s="33"/>
+      <c r="C45" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D45" s="38"/>
       <c r="E45" s="38"/>
       <c r="F45" s="34"/>
@@ -2745,7 +2844,10 @@
       <c r="B46" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="39"/>
+      <c r="C46" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D46" s="44"/>
       <c r="E46" s="44"/>
       <c r="F46" s="41"/>
@@ -2785,7 +2887,10 @@
       <c r="B47" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C47" s="33"/>
+      <c r="C47" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D47" s="38"/>
       <c r="E47" s="38"/>
       <c r="F47" s="34"/>
@@ -2823,7 +2928,10 @@
       <c r="B48" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C48" s="39"/>
+      <c r="C48" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D48" s="44"/>
       <c r="E48" s="44"/>
       <c r="F48" s="41"/>
@@ -2864,127 +2972,127 @@
         <v>51</v>
       </c>
       <c r="C49" s="55">
-        <f t="shared" ref="C49:AG49" si="1">sum(C13,C15,C17,C19,C21,C23,C25,C27,C29,C31,C33,C35,C37,C39,C41,C43,C45,C47)</f>
+        <f t="shared" ref="C49:AG49" si="2">sum(C13,C15,C17,C19,C21,C23,C25,C27,C29,C31,C33,C35,C37,C39,C41,C43,C45,C47)</f>
         <v>0</v>
       </c>
       <c r="D49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Y49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AA49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AC49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AE49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AG49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH49" s="18"/>
@@ -2995,127 +3103,127 @@
         <v>52</v>
       </c>
       <c r="C50" s="57">
-        <f t="shared" ref="C50:AG50" si="2">sum(C14,C16,C18,C20,C22,C24,C26,C28,C30,C32,C34,C36,C38,C40,C42,C44,C46,C48)</f>
+        <f t="shared" ref="C50:AG50" si="3">sum(C14,C16,C18,C20,C22,C24,C26,C28,C30,C32,C34,C36,C38,C40,C42,C44,C46,C48)</f>
         <v>0</v>
       </c>
       <c r="D50" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E50" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F50" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G50" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H50" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I50" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J50" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K50" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L50" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M50" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N50" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O50" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P50" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q50" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R50" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S50" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T50" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U50" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V50" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W50" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="X50" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y50" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Z50" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AA50" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AB50" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC50" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AD50" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE50" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF50" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG50" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AH50" s="18"/>

</xml_diff>